<commit_message>
Tried more model optimisation
</commit_message>
<xml_diff>
--- a/OC Trial/Model_Optimisation.xlsx
+++ b/OC Trial/Model_Optimisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oormi\Desktop\coding\Project4\project4_group3_health_ml\OC Trial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CCFE607-7741-437A-9360-0C443DD3AE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C53D11-631D-47D8-A96E-3B8CC929A1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4572" yWindow="2100" windowWidth="23040" windowHeight="12204" xr2:uid="{2D5A1C5C-38CF-4907-B6EC-545A86749B4C}"/>
+    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{2D5A1C5C-38CF-4907-B6EC-545A86749B4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Model</t>
   </si>
@@ -65,10 +65,34 @@
     <t>Get rid of columns with low feature importance(smoking, diabetes, obesity, alcohol consumption, previous heart problems, medication use, family history, diet, sleep hours per day, physical activity days per week)</t>
   </si>
   <si>
-    <t>Deep learning</t>
-  </si>
-  <si>
     <t>New model type; kept columns from previous iteration</t>
+  </si>
+  <si>
+    <t>Change data types from float to int to reduce the number of unique values</t>
+  </si>
+  <si>
+    <t>Drop 'Sex' and 'Stress Level' columns to reduce user input to 8 features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bin 'age' values </t>
+  </si>
+  <si>
+    <t>ANN</t>
+  </si>
+  <si>
+    <t>Bin all columns except for exercise and sedentary hours per week</t>
+  </si>
+  <si>
+    <t>Same as above but with different model</t>
+  </si>
+  <si>
+    <t>Reduce n(epochs) to 50 and add a third hidden layer</t>
+  </si>
+  <si>
+    <t>Increase n(epochs) to 200 and add more neurons to each hidden layer</t>
+  </si>
+  <si>
+    <t>Use Kerastuner to find the best hyperparameters</t>
   </si>
 </sst>
 </file>
@@ -104,9 +128,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9D7EB3-C444-408F-B1D3-391C54D1A573}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,13 +535,125 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
       </c>
       <c r="D6" s="1">
         <v>0.61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.65300000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimisation tried again; code reorganised
</commit_message>
<xml_diff>
--- a/OC Trial/Model_Optimisation.xlsx
+++ b/OC Trial/Model_Optimisation.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oormi\Desktop\coding\Project4\project4_group3_health_ml\OC Trial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2A1350-97CC-4A39-AE16-2D28A1C2F3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45293AD4-B8BF-41BB-BC1E-32EAB6E00014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{2D5A1C5C-38CF-4907-B6EC-545A86749B4C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Iteration log" sheetId="1" r:id="rId1"/>
+    <sheet name="Confusion matrices" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Model</t>
   </si>
@@ -126,6 +127,36 @@
   </si>
   <si>
     <t>=====================   SWITCH BACK TO REGIONAL DATASET</t>
+  </si>
+  <si>
+    <t>Reduce the number of unique values by converting float columns to integer</t>
+  </si>
+  <si>
+    <t>same-ish as bins; binning not required?</t>
+  </si>
+  <si>
+    <t>Add systolic and diastolic BP</t>
+  </si>
+  <si>
+    <t>similar confusion matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">over-sampling </t>
+  </si>
+  <si>
+    <t>drop in accuracy</t>
+  </si>
+  <si>
+    <t>under-sampling: Near-Miss</t>
+  </si>
+  <si>
+    <t>Even steeper drop in accuracy and recall</t>
+  </si>
+  <si>
+    <t>under-sampling: RandomUnderSampler - majority</t>
+  </si>
+  <si>
+    <t>still poor accuracy and recall; no under-sampling</t>
   </si>
 </sst>
 </file>
@@ -181,6 +212,231 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>22861</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>7619</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>4256</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>18384</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B1A8022-6F95-A5DB-7A76-D2BEF8997FB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4290061" y="190499"/>
+          <a:ext cx="3029395" cy="2205325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>68581</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>64385</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>99887</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22DE812F-AAB7-54D7-72F2-15F02E052DF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="68581" y="247265"/>
+          <a:ext cx="3079306" cy="2069215"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>60961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>2049</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C6D0793-4A65-9081-3F29-18A76A09F913}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="60960" y="3169921"/>
+          <a:ext cx="2994660" cy="1952768"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>608172</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A888F990-1516-A9DB-6723-8FA8AD73A938}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3649980" y="3291840"/>
+          <a:ext cx="3054192" cy="1927860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>138234</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F94C0237-6DCB-D267-6E60-1FF690FF69C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7620" y="5509260"/>
+          <a:ext cx="3017520" cy="1944174"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -480,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9D7EB3-C444-408F-B1D3-391C54D1A573}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,7 +1031,131 @@
         <v>29</v>
       </c>
     </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="E23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="E26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>18</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="E27" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5359FE4-1D78-4170-8DBB-4E154AFB04C3}">
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Random forest has the highest accuracy
</commit_message>
<xml_diff>
--- a/OC Trial/Model_Optimisation.xlsx
+++ b/OC Trial/Model_Optimisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oormi\Desktop\coding\Project4\project4_group3_health_ml\OC Trial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45293AD4-B8BF-41BB-BC1E-32EAB6E00014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F70D98-3FEE-4A1B-B1D6-E716482A4FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{2D5A1C5C-38CF-4907-B6EC-545A86749B4C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t>Model</t>
   </si>
@@ -157,6 +157,21 @@
   </si>
   <si>
     <t>still poor accuracy and recall; no under-sampling</t>
+  </si>
+  <si>
+    <t>same as 15 but with 500 n-estimators</t>
+  </si>
+  <si>
+    <t>good recall for 0; poor for 1</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>same as 19; different model</t>
+  </si>
+  <si>
+    <t>no actual or predicted 1 values; reject model</t>
   </si>
 </sst>
 </file>
@@ -428,6 +443,50 @@
         <a:xfrm>
           <a:off x="7620" y="5509260"/>
           <a:ext cx="3017520" cy="1944174"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>601981</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>435038</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5649A88-6F31-10F4-4BA3-F5E2E78E1116}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3649981" y="5486401"/>
+          <a:ext cx="2881057" cy="1935479"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -736,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9D7EB3-C444-408F-B1D3-391C54D1A573}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1116,6 +1175,40 @@
         <v>39</v>
       </c>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>19</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.63719999999999999</v>
+      </c>
+      <c r="E28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.64180000000000004</v>
+      </c>
+      <c r="E29" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1126,7 +1219,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1153,6 +1246,9 @@
       <c r="A30">
         <v>16</v>
       </c>
+      <c r="G30">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More optimisations to practice model
</commit_message>
<xml_diff>
--- a/OC Trial/Model_Optimisation.xlsx
+++ b/OC Trial/Model_Optimisation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oormi\Desktop\coding\Project4\project4_group3_health_ml\OC Trial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F70D98-3FEE-4A1B-B1D6-E716482A4FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3620A0-9C63-4F3B-A423-4C1273DD74BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{2D5A1C5C-38CF-4907-B6EC-545A86749B4C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
   <si>
     <t>Model</t>
   </si>
@@ -172,6 +172,33 @@
   </si>
   <si>
     <t>no actual or predicted 1 values; reject model</t>
+  </si>
+  <si>
+    <t>hyperparameter tuning</t>
+  </si>
+  <si>
+    <t>bad recall and precision for 1 vals</t>
+  </si>
+  <si>
+    <t>reduce n_estimators to 100</t>
+  </si>
+  <si>
+    <t>Increase class_weight of 1</t>
+  </si>
+  <si>
+    <t>Increased accuracy and precision</t>
+  </si>
+  <si>
+    <t>Implementing threshold of 0.40 and class_weight of 1:20</t>
+  </si>
+  <si>
+    <t>Good recall for slightly lower accuracy</t>
+  </si>
+  <si>
+    <t>threshold = 0.47</t>
+  </si>
+  <si>
+    <t>better recall and precision</t>
   </si>
 </sst>
 </file>
@@ -495,6 +522,182 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>535529</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD1011B4-580D-A742-BE4A-34BDEEBBC317}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7620" y="7924800"/>
+          <a:ext cx="2966309" cy="1912620"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>15241</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>93829</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>133853</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13C32D88-D95D-A91C-B922-54CDEC02F314}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3672841" y="7957669"/>
+          <a:ext cx="2613659" cy="1685944"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>604132</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>4334</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6771A0B7-FAB8-EFB8-D6A8-8F3CB2C52D64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30480" y="10096500"/>
+          <a:ext cx="3012052" cy="1977914"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>62184</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>109149</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F95E39F-A88F-E537-0FB6-FE853971BFDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3665220" y="10120584"/>
+          <a:ext cx="2674620" cy="1875765"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -795,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9D7EB3-C444-408F-B1D3-391C54D1A573}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1209,6 +1412,88 @@
         <v>44</v>
       </c>
     </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="E30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.62919999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>23</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.64180000000000004</v>
+      </c>
+      <c r="E32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>24</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.6321</v>
+      </c>
+      <c r="E33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.62639999999999996</v>
+      </c>
+      <c r="E34" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1216,10 +1501,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5359FE4-1D78-4170-8DBB-4E154AFB04C3}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1250,6 +1535,22 @@
         <v>19</v>
       </c>
     </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>22</v>
+      </c>
+      <c r="G43">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>24</v>
+      </c>
+      <c r="G55">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>